<commit_message>
fix: un solo <h1> por pagina
</commit_message>
<xml_diff>
--- a/src/Head.xlsx
+++ b/src/Head.xlsx
@@ -586,7 +586,7 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>2025-10-02T10:23:34-05:00</t>
+    <t>2025-10-08T11:11:03-05:00</t>
   </si>
   <si>
     <t>&lt;?xml version='1.0' encoding='UTF-8'?&gt;</t>
@@ -32780,11 +32780,11 @@
     <row r="6" spans="1:5">
       <c r="A6" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B6,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B6" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C6" s="111"/>
       <c r="E6" s="110"/>
@@ -32851,11 +32851,11 @@
     <row r="13" spans="1:5">
       <c r="A13" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B13,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B13" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C13" s="111"/>
       <c r="E13" s="110"/>
@@ -32915,11 +32915,11 @@
     <row r="19" spans="1:5">
       <c r="A19" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B19,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B19" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C19" s="111"/>
       <c r="E19" s="110"/>
@@ -32979,11 +32979,11 @@
     <row r="25" spans="1:5">
       <c r="A25" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B25,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B25" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C25" s="111"/>
       <c r="E25" s="110"/>
@@ -33043,11 +33043,11 @@
     <row r="31" spans="1:5">
       <c r="A31" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B31,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B31" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C31" s="111"/>
       <c r="E31" s="110"/>
@@ -33107,11 +33107,11 @@
     <row r="37" spans="1:5">
       <c r="A37" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B37,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B37" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C37" s="111"/>
       <c r="E37" s="110"/>
@@ -33171,11 +33171,11 @@
     <row r="43" spans="1:5">
       <c r="A43" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B43,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B43" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C43" s="111"/>
       <c r="E43" s="110"/>
@@ -33235,11 +33235,11 @@
     <row r="49" spans="1:5">
       <c r="A49" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B49,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B49" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C49" s="111"/>
       <c r="E49" s="110"/>
@@ -33299,11 +33299,11 @@
     <row r="55" spans="1:5">
       <c r="A55" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B55,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B55" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C55" s="111"/>
       <c r="E55" s="110"/>
@@ -33371,11 +33371,11 @@
     <row r="62" spans="1:5">
       <c r="A62" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B62,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B62" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C62" s="111"/>
       <c r="E62" s="110"/>
@@ -33435,11 +33435,11 @@
     <row r="68" spans="1:5">
       <c r="A68" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B68,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B68" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C68" s="111"/>
       <c r="E68" s="110"/>
@@ -33507,11 +33507,11 @@
     <row r="75" spans="1:5">
       <c r="A75" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B75,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B75" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C75" s="111"/>
       <c r="E75" s="110"/>
@@ -33571,11 +33571,11 @@
     <row r="81" spans="1:5">
       <c r="A81" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B81,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B81" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C81" s="111"/>
       <c r="E81" s="110"/>
@@ -33635,11 +33635,11 @@
     <row r="87" spans="1:5">
       <c r="A87" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B87,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B87" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C87" s="111"/>
       <c r="E87" s="110"/>
@@ -33699,11 +33699,11 @@
     <row r="93" spans="1:5">
       <c r="A93" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B93,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B93" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C93" s="111"/>
       <c r="E93" s="110"/>
@@ -33762,11 +33762,11 @@
     <row r="99" spans="1:5">
       <c r="A99" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B99,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B99" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C99" s="111"/>
       <c r="E99" s="110"/>
@@ -33826,11 +33826,11 @@
     <row r="105" spans="1:5">
       <c r="A105" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B105,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B105" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C105" s="111"/>
       <c r="E105" s="110"/>
@@ -33898,11 +33898,11 @@
     <row r="112" spans="1:5">
       <c r="A112" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B112,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B112" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C112" s="111"/>
       <c r="E112" s="110"/>
@@ -33964,11 +33964,11 @@
     <row r="118" spans="1:5">
       <c r="A118" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B118,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B118" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C118" s="111"/>
       <c r="E118" s="110"/>
@@ -34036,11 +34036,11 @@
     <row r="125" spans="1:5">
       <c r="A125" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B125,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B125" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C125" s="111"/>
       <c r="E125" s="110"/>
@@ -34100,11 +34100,11 @@
     <row r="131" spans="1:5">
       <c r="A131" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B131,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B131" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C131" s="111"/>
       <c r="E131" s="110"/>
@@ -34164,11 +34164,11 @@
     <row r="137" spans="1:5">
       <c r="A137" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B137,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B137" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C137" s="111"/>
       <c r="E137" s="110"/>
@@ -34228,11 +34228,11 @@
     <row r="143" spans="1:5">
       <c r="A143" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B143,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B143" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C143" s="111"/>
       <c r="E143" s="110"/>
@@ -34292,11 +34292,11 @@
     <row r="149" spans="1:5">
       <c r="A149" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B149,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B149" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C149" s="111"/>
       <c r="E149" s="110"/>
@@ -34356,11 +34356,11 @@
     <row r="155" spans="1:5">
       <c r="A155" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B155,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B155" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C155" s="111"/>
       <c r="E155" s="110"/>
@@ -34420,11 +34420,11 @@
     <row r="161" spans="1:5">
       <c r="A161" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B161,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B161" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C161" s="111"/>
       <c r="E161" s="110"/>
@@ -34484,11 +34484,11 @@
     <row r="167" spans="1:5">
       <c r="A167" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B167,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B167" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C167" s="111"/>
       <c r="E167" s="110"/>
@@ -34548,11 +34548,11 @@
     <row r="173" spans="1:5">
       <c r="A173" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B173,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B173" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C173" s="111"/>
       <c r="E173" s="110"/>
@@ -34612,11 +34612,11 @@
     <row r="179" spans="1:5">
       <c r="A179" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B179,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B179" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C179" s="111"/>
       <c r="E179" s="110"/>
@@ -34676,11 +34676,11 @@
     <row r="185" spans="1:5">
       <c r="A185" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B185,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B185" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C185" s="111"/>
       <c r="E185" s="110"/>
@@ -34740,11 +34740,11 @@
     <row r="191" spans="1:5">
       <c r="A191" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B191,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B191" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C191" s="111"/>
       <c r="E191" s="110"/>
@@ -34804,11 +34804,11 @@
     <row r="197" spans="1:5">
       <c r="A197" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B197,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B197" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C197" s="111"/>
       <c r="E197" s="110"/>
@@ -34868,11 +34868,11 @@
     <row r="203" spans="1:5">
       <c r="A203" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B203,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B203" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C203" s="111"/>
       <c r="E203" s="110"/>
@@ -34932,11 +34932,11 @@
     <row r="209" spans="1:5">
       <c r="A209" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B209,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B209" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C209" s="111"/>
       <c r="E209" s="110"/>
@@ -34995,11 +34995,11 @@
     <row r="215" spans="1:5">
       <c r="A215" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B215,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B215" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C215" s="111"/>
       <c r="E215" s="110"/>
@@ -35067,11 +35067,11 @@
     <row r="222" spans="1:5">
       <c r="A222" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B222,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B222" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C222" s="111"/>
       <c r="E222" s="110"/>
@@ -35137,11 +35137,11 @@
     <row r="229" spans="1:5">
       <c r="A229" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B229,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B229" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C229" s="111"/>
       <c r="E229" s="110"/>
@@ -35209,11 +35209,11 @@
     <row r="236" spans="1:5">
       <c r="A236" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B236,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B236" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C236" s="111"/>
       <c r="E236" s="110"/>
@@ -35273,11 +35273,11 @@
     <row r="242" spans="1:5">
       <c r="A242" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B242,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B242" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C242" s="111"/>
       <c r="E242" s="110"/>
@@ -35337,11 +35337,11 @@
     <row r="248" spans="1:5">
       <c r="A248" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B248,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B248" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C248" s="111"/>
       <c r="E248" s="110"/>
@@ -35401,11 +35401,11 @@
     <row r="254" spans="1:5">
       <c r="A254" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B254,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B254" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C254" s="111"/>
       <c r="E254" s="110"/>
@@ -35465,11 +35465,11 @@
     <row r="260" spans="1:5">
       <c r="A260" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B260,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B260" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C260" s="111"/>
       <c r="E260" s="110"/>
@@ -35529,11 +35529,11 @@
     <row r="266" spans="1:5">
       <c r="A266" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B266,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B266" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C266" s="111"/>
       <c r="E266" s="110"/>
@@ -35593,11 +35593,11 @@
     <row r="272" spans="1:5">
       <c r="A272" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B272,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B272" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C272" s="111"/>
       <c r="E272" s="110"/>
@@ -35657,11 +35657,11 @@
     <row r="278" spans="1:5">
       <c r="A278" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B278,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B278" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C278" s="111"/>
       <c r="E278" s="110"/>
@@ -35721,11 +35721,11 @@
     <row r="284" spans="1:5">
       <c r="A284" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B284,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B284" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C284" s="111"/>
       <c r="E284" s="110"/>
@@ -35785,11 +35785,11 @@
     <row r="290" spans="1:5">
       <c r="A290" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B290,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B290" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C290" s="111"/>
       <c r="E290" s="110"/>
@@ -35849,11 +35849,11 @@
     <row r="296" spans="1:5">
       <c r="A296" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B296,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B296" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C296" s="111"/>
       <c r="E296" s="110"/>
@@ -35913,11 +35913,11 @@
     <row r="302" spans="1:5">
       <c r="A302" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B302,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B302" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C302" s="111"/>
       <c r="E302" s="110"/>
@@ -35977,11 +35977,11 @@
     <row r="308" spans="1:5">
       <c r="A308" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B308,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B308" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C308" s="111"/>
       <c r="E308" s="110"/>
@@ -36041,11 +36041,11 @@
     <row r="314" spans="1:5">
       <c r="A314" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B314,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B314" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C314" s="111"/>
       <c r="E314" s="110"/>
@@ -36105,11 +36105,11 @@
     <row r="320" spans="1:5">
       <c r="A320" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B320,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B320" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C320" s="111"/>
       <c r="E320" s="110"/>
@@ -36169,11 +36169,11 @@
     <row r="326" spans="1:5">
       <c r="A326" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B326,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B326" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C326" s="111"/>
       <c r="E326" s="110"/>
@@ -36233,11 +36233,11 @@
     <row r="332" spans="1:5">
       <c r="A332" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B332,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B332" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C332" s="111"/>
       <c r="E332" s="110"/>
@@ -36297,11 +36297,11 @@
     <row r="338" spans="1:5">
       <c r="A338" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B338,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B338" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C338" s="111"/>
       <c r="E338" s="110"/>
@@ -36361,11 +36361,11 @@
     <row r="344" spans="1:5">
       <c r="A344" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B344,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B344" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C344" s="111"/>
       <c r="E344" s="110"/>
@@ -36425,11 +36425,11 @@
     <row r="350" spans="1:5">
       <c r="A350" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B350,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B350" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C350" s="111"/>
       <c r="E350" s="110"/>
@@ -36489,11 +36489,11 @@
     <row r="356" spans="1:5">
       <c r="A356" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B356,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B356" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C356" s="111"/>
       <c r="E356" s="110"/>
@@ -36553,11 +36553,11 @@
     <row r="362" spans="1:5">
       <c r="A362" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B362,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B362" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C362" s="111"/>
       <c r="E362" s="110"/>
@@ -36617,11 +36617,11 @@
     <row r="368" spans="1:5">
       <c r="A368" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B368,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B368" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C368" s="111"/>
       <c r="E368" s="110"/>
@@ -36681,11 +36681,11 @@
     <row r="374" spans="1:5">
       <c r="A374" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B374,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B374" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C374" s="111"/>
       <c r="E374" s="110"/>
@@ -36745,11 +36745,11 @@
     <row r="380" spans="1:5">
       <c r="A380" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B380,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B380" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C380" s="111"/>
       <c r="E380" s="110"/>
@@ -36809,11 +36809,11 @@
     <row r="386" spans="1:5">
       <c r="A386" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B386,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B386" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C386" s="111"/>
       <c r="E386" s="110"/>
@@ -36873,11 +36873,11 @@
     <row r="392" spans="1:5">
       <c r="A392" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B392,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B392" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C392" s="111"/>
       <c r="E392" s="110"/>
@@ -36937,11 +36937,11 @@
     <row r="398" spans="1:5">
       <c r="A398" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B398,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B398" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C398" s="111"/>
       <c r="E398" s="110"/>
@@ -37001,11 +37001,11 @@
     <row r="404" spans="1:5">
       <c r="A404" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B404,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B404" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C404" s="111"/>
       <c r="E404" s="110"/>
@@ -37065,11 +37065,11 @@
     <row r="410" spans="1:5">
       <c r="A410" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B410,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B410" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C410" s="111"/>
       <c r="E410" s="110"/>
@@ -37129,11 +37129,11 @@
     <row r="416" spans="1:5">
       <c r="A416" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B416,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B416" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C416" s="111"/>
       <c r="E416" s="110"/>
@@ -37193,11 +37193,11 @@
     <row r="422" spans="1:5">
       <c r="A422" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B422,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B422" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C422" s="111"/>
       <c r="E422" s="110"/>
@@ -37257,11 +37257,11 @@
     <row r="428" spans="1:5">
       <c r="A428" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B428,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B428" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C428" s="111"/>
       <c r="E428" s="110"/>
@@ -37321,11 +37321,11 @@
     <row r="434" spans="1:5">
       <c r="A434" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B434,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B434" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C434" s="111"/>
       <c r="E434" s="110"/>
@@ -37385,11 +37385,11 @@
     <row r="440" spans="1:5">
       <c r="A440" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B440,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B440" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C440" s="111"/>
       <c r="E440" s="110"/>
@@ -37449,11 +37449,11 @@
     <row r="446" spans="1:5">
       <c r="A446" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B446,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B446" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C446" s="111"/>
       <c r="E446" s="110"/>
@@ -37513,11 +37513,11 @@
     <row r="452" spans="1:5">
       <c r="A452" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B452,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B452" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C452" s="111"/>
       <c r="E452" s="110"/>
@@ -37576,11 +37576,11 @@
     <row r="458" spans="1:3">
       <c r="A458" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B458,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B458" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C458" s="111"/>
     </row>
@@ -37645,11 +37645,11 @@
     <row r="465" spans="1:5">
       <c r="A465" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B465,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B465" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C465" s="111"/>
       <c r="E465" s="110"/>
@@ -37709,11 +37709,11 @@
     <row r="471" spans="1:5">
       <c r="A471" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B471,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B471" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C471" s="111"/>
       <c r="E471" s="110"/>
@@ -37773,11 +37773,11 @@
     <row r="477" spans="1:5">
       <c r="A477" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B477,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B477" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C477" s="111"/>
       <c r="E477" s="110"/>
@@ -37837,11 +37837,11 @@
     <row r="483" spans="1:5">
       <c r="A483" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B483,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B483" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C483" s="111"/>
       <c r="E483" s="110"/>
@@ -37901,11 +37901,11 @@
     <row r="489" spans="1:5">
       <c r="A489" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B489,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B489" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C489" s="111"/>
       <c r="E489" s="110"/>
@@ -37965,11 +37965,11 @@
     <row r="495" spans="1:5">
       <c r="A495" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B495,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B495" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C495" s="111"/>
       <c r="E495" s="110"/>
@@ -38029,11 +38029,11 @@
     <row r="501" spans="1:5">
       <c r="A501" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B501,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B501" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C501" s="111"/>
       <c r="E501" s="110"/>
@@ -38093,11 +38093,11 @@
     <row r="507" spans="1:5">
       <c r="A507" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B507,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B507" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C507" s="111"/>
       <c r="E507" s="110"/>
@@ -38157,11 +38157,11 @@
     <row r="513" spans="1:5">
       <c r="A513" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B513,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B513" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C513" s="111"/>
       <c r="E513" s="110"/>
@@ -38221,11 +38221,11 @@
     <row r="519" spans="1:5">
       <c r="A519" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B519,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B519" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C519" s="111"/>
       <c r="E519" s="110"/>
@@ -38285,11 +38285,11 @@
     <row r="525" spans="1:5">
       <c r="A525" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B525,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B525" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C525" s="111"/>
       <c r="E525" s="110"/>
@@ -38349,11 +38349,11 @@
     <row r="531" spans="1:5">
       <c r="A531" s="107" t="str">
         <f>CONCATENATE("&lt;lastmod&gt;",B531,"&lt;/lastmod&gt;")</f>
-        <v>&lt;lastmod&gt;2025-10-02T10:23:34-05:00&lt;/lastmod&gt;</v>
+        <v>&lt;lastmod&gt;2025-10-08T11:11:03-05:00&lt;/lastmod&gt;</v>
       </c>
       <c r="B531" s="108" t="str">
         <f>$C$1</f>
-        <v>2025-10-02T10:23:34-05:00</v>
+        <v>2025-10-08T11:11:03-05:00</v>
       </c>
       <c r="C531" s="111"/>
       <c r="E531" s="110"/>

</xml_diff>